<commit_message>
Update Evaluation of CNN Model.xlsx
</commit_message>
<xml_diff>
--- a/CNN FInal Project/Evaluation of CNN Model.xlsx
+++ b/CNN FInal Project/Evaluation of CNN Model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owens\OneDrive\Documents\GitHub\NeuralNetwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owens\OneDrive\Documents\GitHub\NeuralNetwork\CNN FInal Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C6DC44-4246-4A2F-849D-C7D27F6D90C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88025A3-06C6-40C1-8FDD-5FFA8617DC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E858EE2A-F882-4FE9-AFBB-C069914F8F1C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>Car</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Original Model</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -183,6 +186,9 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,30 +504,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB50172-7C8E-4294-B1EE-8FEBB26AB0FE}">
-  <dimension ref="B2:K14"/>
+  <dimension ref="B3:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B3" sqref="B3:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="12" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="3" spans="2:10" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
@@ -531,17 +536,23 @@
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -554,20 +565,23 @@
       <c r="E4" s="2">
         <v>0.32500000000000001</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="H4" s="2">
+        <v>0.55400000000000005</v>
+      </c>
       <c r="I4" s="2">
-        <v>0.55400000000000005</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="J4" s="2">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="K4" s="2">
         <v>0.63100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,20 +594,23 @@
       <c r="E5" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="F5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="H5" s="2">
+        <v>0.84</v>
+      </c>
       <c r="I5" s="2">
-        <v>0.84</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="J5" s="2">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="K5" s="2">
         <v>0.872</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" ht="12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -606,20 +623,23 @@
       <c r="E6" s="2">
         <v>0.217</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="H6" s="2">
+        <v>0.51800000000000002</v>
+      </c>
       <c r="I6" s="2">
-        <v>0.51800000000000002</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="J6" s="2">
-        <v>0.61199999999999999</v>
-      </c>
-      <c r="K6" s="2">
         <v>0.56100000000000005</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -632,20 +652,23 @@
       <c r="E7" s="2">
         <v>0.33900000000000002</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="F7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H7" s="2">
+        <v>0.70699999999999996</v>
+      </c>
       <c r="I7" s="2">
-        <v>0.70699999999999996</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="J7" s="2">
-        <v>0.70099999999999996</v>
-      </c>
-      <c r="K7" s="2">
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -658,20 +681,23 @@
       <c r="E8" s="2">
         <v>0.441</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="F8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H8" s="2">
+        <v>0.67600000000000005</v>
+      </c>
       <c r="I8" s="2">
-        <v>0.67600000000000005</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="J8" s="2">
-        <v>0.64100000000000001</v>
-      </c>
-      <c r="K8" s="2">
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" ht="12" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -684,20 +710,23 @@
       <c r="E9" s="2">
         <v>0.55900000000000005</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="F9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H9" s="2">
+        <v>0.81699999999999995</v>
+      </c>
       <c r="I9" s="2">
-        <v>0.81699999999999995</v>
+        <v>0.79900000000000004</v>
       </c>
       <c r="J9" s="2">
-        <v>0.79900000000000004</v>
-      </c>
-      <c r="K9" s="2">
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" ht="12" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -710,20 +739,23 @@
       <c r="E10" s="2">
         <v>0.51</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="F10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H10" s="2">
+        <v>0.85699999999999998</v>
+      </c>
       <c r="I10" s="2">
-        <v>0.85699999999999998</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="J10" s="2">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="K10" s="2">
         <v>0.77700000000000002</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="12" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,20 +768,23 @@
       <c r="E11" s="2">
         <v>0.496</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="H11" s="2">
+        <v>0.75600000000000001</v>
+      </c>
       <c r="I11" s="2">
-        <v>0.75600000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="J11" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="K11" s="2">
         <v>0.77700000000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -762,20 +797,23 @@
       <c r="E12" s="2">
         <v>0.54700000000000004</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="F12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="H12" s="2">
+        <v>0.88400000000000001</v>
+      </c>
       <c r="I12" s="2">
-        <v>0.88400000000000001</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="J12" s="2">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="K12" s="2">
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -788,20 +826,23 @@
       <c r="E13" s="2">
         <v>0.48199999999999998</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H13" s="2">
+        <v>0.86799999999999999</v>
+      </c>
       <c r="I13" s="2">
-        <v>0.86799999999999999</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="J13" s="2">
-        <v>0.79600000000000004</v>
-      </c>
-      <c r="K13" s="2">
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
@@ -814,22 +855,25 @@
       <c r="E14" s="5">
         <v>0.45</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="F14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="H14" s="5">
+        <v>0.748</v>
+      </c>
       <c r="I14" s="5">
-        <v>0.748</v>
+        <v>0.747</v>
       </c>
       <c r="J14" s="5">
-        <v>0.747</v>
-      </c>
-      <c r="K14" s="5">
         <v>0.74399999999999999</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H4:H13">
-    <sortCondition ref="H4:H13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G4:G13">
+    <sortCondition ref="G4:G13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>